<commit_message>
Edits made to file and directory names
Due to \n detecting as line break in Psychopy
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ram\OneDrive - University of Sussex\Desktop\LZ correlation\LZ_correlation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{FFC62BCF-ABD7-4CBA-A36A-D29C909D25BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AAB2856D-6E8D-4CD1-8B9F-54B723B681F5}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{FFC62BCF-ABD7-4CBA-A36A-D29C909D25BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0D7C42FD-A71A-4994-B457-ECBD9C809E91}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>trial</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>image3</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>C:\LZ\natural\natural_119.jpg</t>
   </si>
 </sst>
 </file>
@@ -899,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,7 +919,7 @@
     <col min="5" max="5" width="57.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -929,8 +935,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -946,8 +955,11 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -970,6 +982,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031167D602857F849923F99C158CB76F9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2481ad6f2fc887a8ee6391bf7dc84b15">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e4665a5-634c-44ba-a715-bfb63f053b30" xmlns:ns4="f66be614-e68b-42e6-ba40-e6a67b243d58" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d339bd1eb068684f2c3c72074c527cf" ns3:_="" ns4:_="">
     <xsd:import namespace="0e4665a5-634c-44ba-a715-bfb63f053b30"/>
@@ -1192,15 +1213,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1208,6 +1220,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B618C80D-67DB-4A9D-A924-CFAD03AB4175}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD927C3-3F40-406F-ADBC-3EA3EB9FB41E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1222,14 +1242,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B618C80D-67DB-4A9D-A924-CFAD03AB4175}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>